<commit_message>
EPBDS: added map nulls and map empty strings features support
</commit_message>
<xml_diff>
--- a/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/emptysource/EmptySourceTest.xlsx
+++ b/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/emptysource/EmptySourceTest.xlsx
@@ -174,13 +174,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -480,7 +480,7 @@
   <dimension ref="C4:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -492,13 +492,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:7">
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="3:7">
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -506,31 +506,31 @@
       </c>
     </row>
     <row r="6" spans="3:7">
-      <c r="C6" s="6"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="3:7">
-      <c r="C7" s="6"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="3:7">
-      <c r="C8" s="6"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="3:7">
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="3:7">
       <c r="C13" s="2" t="s">

</xml_diff>